<commit_message>
Se agrega el mensaje en el main
</commit_message>
<xml_diff>
--- a/naves_espaciales.xlsx
+++ b/naves_espaciales.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,22 +461,222 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>lanzadera</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>eeuu</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>saturno v</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>1967</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>tripulada</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>rusia</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>soyus</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1967</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>lanzadera</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>eeuu</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>atlas</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>tripulada</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>shenzou</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>no tripulada</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>rusia</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>luna I</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1959</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>no tripulada</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>europa</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>soho</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1995</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>lanzadera</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>eeuu</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>zenit II</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1985</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>tripulada</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>eeuu</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>apolo</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1966</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>no tripulada</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>eeuu</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>mariner x</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1973</t>
         </is>
       </c>
     </row>

</xml_diff>